<commit_message>
added new whatsapp web py file for sending messages
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="My Sheet One" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,15 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t xml:space="preserve">Hello world</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sidhwa JIIT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">temp</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+  <si>
+    <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enquiry For</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enquiry From</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lv Enterprises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soft Toys</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trade India</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shilpi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LV T</t>
   </si>
 </sst>
 </file>
@@ -104,63 +131,105 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17.32421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>917570090256</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>0</v>
+      <c r="A2" s="1" t="n">
+        <v>7503085792</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>2</v>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>9870117763</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>